<commit_message>
upload carousel and images
</commit_message>
<xml_diff>
--- a/DivisionOfWorl_BC35E_BTcapstone_Hau&Lanh.xlsx
+++ b/DivisionOfWorl_BC35E_BTcapstone_Hau&Lanh.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
   <si>
     <t>Tasks Name</t>
   </si>
@@ -64,13 +64,19 @@
     <t>carousel</t>
   </si>
   <si>
+    <t>17/8/2022</t>
+  </si>
+  <si>
+    <t>18/8/2022</t>
+  </si>
+  <si>
+    <t>service</t>
+  </si>
+  <si>
     <t>Dev A</t>
   </si>
   <si>
     <t>Nhật Trường</t>
-  </si>
-  <si>
-    <t>service</t>
   </si>
   <si>
     <t>welcome</t>
@@ -108,10 +114,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="178" formatCode="[$-409]d\-mmm;@"/>
   </numFmts>
   <fonts count="27">
@@ -138,7 +144,7 @@
     </font>
     <font>
       <b/>
-      <sz val="9"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="1"/>
@@ -152,71 +158,79 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <sz val="9"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="1"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -253,22 +267,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -285,6 +283,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
@@ -292,23 +298,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -359,181 +365,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -668,6 +674,24 @@
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -687,17 +711,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -737,15 +750,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -763,24 +767,26 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -790,134 +796,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="32" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="12" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="28" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
@@ -940,25 +946,28 @@
     <xf numFmtId="9" fontId="4" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="5" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="5" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="5" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -967,7 +976,7 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1310,7 +1319,7 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1354,7 +1363,7 @@
       <c r="I1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="J1" s="22" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1375,260 +1384,264 @@
         <v>11</v>
       </c>
       <c r="F2" s="9"/>
-      <c r="G2" s="6">
+      <c r="G2" s="10">
         <v>44909</v>
       </c>
-      <c r="H2" s="10">
+      <c r="H2" s="11">
         <v>1</v>
       </c>
       <c r="I2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="22"/>
+      <c r="J2" s="23"/>
     </row>
     <row r="3" ht="23.25" customHeight="1" spans="1:10">
       <c r="A3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="11">
+      <c r="B3" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="12">
+        <v>1</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="9"/>
+      <c r="G3" s="10">
+        <v>44909</v>
+      </c>
+      <c r="H3" s="12">
         <v>0.5</v>
       </c>
-      <c r="E3" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="9"/>
-      <c r="G3" s="6">
-        <v>44909</v>
-      </c>
-      <c r="H3" s="11">
-        <v>0.5</v>
-      </c>
       <c r="I3" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="J3" s="22"/>
+        <v>12</v>
+      </c>
+      <c r="J3" s="23"/>
     </row>
     <row r="4" ht="24.75" customHeight="1" spans="1:10">
       <c r="A4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="10">
         <v>44704</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="10">
         <v>44743</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="13">
         <v>0.9</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F4" s="9"/>
-      <c r="G4" s="6">
+      <c r="G4" s="10">
         <v>44909</v>
       </c>
-      <c r="H4" s="12">
+      <c r="H4" s="13">
         <v>0.9</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="J4" s="22"/>
+        <v>18</v>
+      </c>
+      <c r="J4" s="23"/>
     </row>
     <row r="5" ht="21.75" customHeight="1" spans="1:10">
       <c r="A5" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="6">
+        <v>19</v>
+      </c>
+      <c r="B5" s="10">
         <v>44704</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="10">
         <v>44712</v>
       </c>
       <c r="D5" s="7">
         <v>1</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F5" s="9"/>
-      <c r="G5" s="6">
+      <c r="G5" s="10">
         <v>44909</v>
       </c>
       <c r="H5" s="7">
         <v>1</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="J5" s="22"/>
+        <v>18</v>
+      </c>
+      <c r="J5" s="23"/>
     </row>
     <row r="6" ht="22.5" customHeight="1" spans="1:10">
       <c r="A6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="10">
+        <v>44732</v>
+      </c>
+      <c r="C6" s="10">
+        <v>44740</v>
+      </c>
+      <c r="D6" s="13">
+        <v>0.9</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="9"/>
+      <c r="G6" s="10">
+        <v>44909</v>
+      </c>
+      <c r="H6" s="13">
+        <v>0.9</v>
+      </c>
+      <c r="I6" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="6">
-        <v>44732</v>
-      </c>
-      <c r="C6" s="6">
-        <v>44740</v>
-      </c>
-      <c r="D6" s="12">
-        <v>0.9</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="9"/>
-      <c r="G6" s="6">
-        <v>44909</v>
-      </c>
-      <c r="H6" s="12">
-        <v>0.9</v>
-      </c>
-      <c r="I6" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="J6" s="22"/>
+      <c r="J6" s="23"/>
     </row>
     <row r="7" ht="24.75" customHeight="1" spans="1:10">
       <c r="A7" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="6">
+        <v>21</v>
+      </c>
+      <c r="B7" s="10">
         <v>44737</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="10">
         <v>44743</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="13">
         <v>0.8</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F7" s="9"/>
-      <c r="G7" s="6">
+      <c r="G7" s="10">
         <v>44909</v>
       </c>
-      <c r="H7" s="12">
+      <c r="H7" s="13">
         <v>0.8</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="J7" s="22"/>
+        <v>18</v>
+      </c>
+      <c r="J7" s="23"/>
     </row>
     <row r="8" ht="22.5" customHeight="1" spans="1:10">
       <c r="A8" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="6">
+        <v>22</v>
+      </c>
+      <c r="B8" s="10">
         <v>44905</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="10">
         <v>44908</v>
       </c>
       <c r="D8" s="7">
         <v>1</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F8" s="9"/>
-      <c r="G8" s="6">
+      <c r="G8" s="10">
         <v>44909</v>
       </c>
       <c r="H8" s="7">
         <v>1</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="J8" s="22"/>
+        <v>24</v>
+      </c>
+      <c r="J8" s="23"/>
     </row>
     <row r="9" ht="25.5" customHeight="1" spans="1:10">
       <c r="A9" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
-      <c r="D9" s="13"/>
+      <c r="D9" s="14"/>
       <c r="E9" s="8"/>
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
-      <c r="H9" s="13"/>
+      <c r="H9" s="14"/>
       <c r="I9" s="8"/>
-      <c r="J9" s="22"/>
+      <c r="J9" s="23"/>
     </row>
     <row r="10" ht="24" customHeight="1" spans="1:10">
       <c r="A10" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
-      <c r="D10" s="13"/>
+      <c r="D10" s="14"/>
       <c r="E10" s="8"/>
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
-      <c r="H10" s="13"/>
+      <c r="H10" s="14"/>
       <c r="I10" s="8"/>
-      <c r="J10" s="22"/>
+      <c r="J10" s="23"/>
     </row>
     <row r="11" ht="24" customHeight="1" spans="1:10">
       <c r="A11" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
-      <c r="D11" s="13"/>
+      <c r="D11" s="14"/>
       <c r="E11" s="8"/>
       <c r="F11" s="9"/>
       <c r="G11" s="9"/>
-      <c r="H11" s="13"/>
+      <c r="H11" s="14"/>
       <c r="I11" s="8"/>
-      <c r="J11" s="22"/>
+      <c r="J11" s="23"/>
     </row>
     <row r="12" ht="21" customHeight="1" spans="1:10">
       <c r="A12" s="4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
-      <c r="D12" s="13"/>
+      <c r="D12" s="14"/>
       <c r="E12" s="9"/>
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
-      <c r="H12" s="13"/>
+      <c r="H12" s="14"/>
       <c r="I12" s="8"/>
-      <c r="J12" s="22"/>
+      <c r="J12" s="23"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="14"/>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="23"/>
-      <c r="J13" s="18"/>
+      <c r="A13" s="15"/>
+      <c r="B13" s="16"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="24"/>
+      <c r="J13" s="19"/>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="17"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="19"/>
-      <c r="I14" s="20"/>
-      <c r="J14" s="18"/>
+      <c r="A14" s="18"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix and upload header
</commit_message>
<xml_diff>
--- a/DivisionOfWorl_BC35E_BTcapstone_Hau&Lanh.xlsx
+++ b/DivisionOfWorl_BC35E_BTcapstone_Hau&Lanh.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
   <si>
     <t>Tasks Name</t>
   </si>
@@ -61,24 +61,27 @@
     <t>Nguyễn Văn Lanh</t>
   </si>
   <si>
+    <t>header</t>
+  </si>
+  <si>
+    <t>17/8/2022</t>
+  </si>
+  <si>
+    <t>18/8/2022</t>
+  </si>
+  <si>
     <t>carousel</t>
   </si>
   <si>
-    <t>17/8/2022</t>
-  </si>
-  <si>
-    <t>18/8/2022</t>
+    <t>Dev A</t>
+  </si>
+  <si>
+    <t>Nhật Trường</t>
   </si>
   <si>
     <t>service</t>
   </si>
   <si>
-    <t>Dev A</t>
-  </si>
-  <si>
-    <t>Nhật Trường</t>
-  </si>
-  <si>
     <t>welcome</t>
   </si>
   <si>
@@ -88,13 +91,13 @@
     <t>learn</t>
   </si>
   <si>
+    <t>Dev1</t>
+  </si>
+  <si>
+    <t>Dev2</t>
+  </si>
+  <si>
     <t>numbers</t>
-  </si>
-  <si>
-    <t>Dev1</t>
-  </si>
-  <si>
-    <t>Dev2</t>
   </si>
   <si>
     <t>feedback</t>
@@ -114,10 +117,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="178" formatCode="[$-409]d\-mmm;@"/>
   </numFmts>
   <fonts count="27">
@@ -176,6 +179,22 @@
       <charset val="1"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -184,22 +203,53 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -213,60 +263,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -298,6 +294,20 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -308,13 +318,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -365,6 +368,30 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -377,7 +404,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -389,19 +512,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -419,48 +536,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -468,78 +543,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -595,7 +598,7 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
+        <color rgb="FFCCCCCC"/>
       </left>
       <right style="thin">
         <color rgb="FF000000"/>
@@ -608,7 +611,7 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFCCCCCC"/>
+        <color rgb="FF000000"/>
       </left>
       <right style="thin">
         <color rgb="FF000000"/>
@@ -621,7 +624,7 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
+        <color rgb="FFCCCCCC"/>
       </left>
       <right style="thin">
         <color rgb="FF000000"/>
@@ -636,7 +639,7 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFCCCCCC"/>
+        <color rgb="FF000000"/>
       </left>
       <right style="thin">
         <color rgb="FF000000"/>
@@ -682,16 +685,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -711,6 +705,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -726,15 +729,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -750,6 +744,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -796,130 +799,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="28" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -967,25 +970,25 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -994,7 +997,7 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -1316,10 +1319,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1619,29 +1622,34 @@
       <c r="I12" s="8"/>
       <c r="J12" s="23"/>
     </row>
-    <row r="13" spans="1:10">
-      <c r="A13" s="15"/>
-      <c r="B13" s="16"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="17"/>
+    <row r="13" ht="19" customHeight="1" spans="1:10">
+      <c r="A13" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="16"/>
       <c r="I13" s="24"/>
-      <c r="J13" s="19"/>
+      <c r="J13" s="18"/>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="18"/>
-      <c r="B14" s="19"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="20"/>
-      <c r="I14" s="21"/>
-      <c r="J14" s="19"/>
+      <c r="A14" s="17"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="19"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="18"/>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix and up load carousel
</commit_message>
<xml_diff>
--- a/DivisionOfWorl_BC35E_BTcapstone_Hau&Lanh.xlsx
+++ b/DivisionOfWorl_BC35E_BTcapstone_Hau&Lanh.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
   <si>
     <t>Tasks Name</t>
   </si>
@@ -73,13 +73,16 @@
     <t>carousel</t>
   </si>
   <si>
+    <t>19/8/2022</t>
+  </si>
+  <si>
+    <t>service</t>
+  </si>
+  <si>
     <t>Dev A</t>
   </si>
   <si>
     <t>Nhật Trường</t>
-  </si>
-  <si>
-    <t>service</t>
   </si>
   <si>
     <t>welcome</t>
@@ -117,10 +120,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="178" formatCode="[$-409]d\-mmm;@"/>
   </numFmts>
   <fonts count="27">
@@ -180,76 +183,31 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -263,16 +221,53 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="15"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -281,6 +276,29 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -288,29 +306,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -368,85 +371,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -458,73 +527,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -681,11 +684,65 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -707,69 +764,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -778,10 +772,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -799,22 +802,28 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -823,106 +832,100 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="20" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1322,7 +1325,7 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1430,17 +1433,17 @@
       <c r="A4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="10">
-        <v>44704</v>
-      </c>
-      <c r="C4" s="10">
-        <v>44743</v>
+      <c r="B4" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>17</v>
       </c>
       <c r="D4" s="13">
         <v>0.9</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="F4" s="9"/>
       <c r="G4" s="10">
@@ -1450,13 +1453,13 @@
         <v>0.9</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="J4" s="23"/>
     </row>
     <row r="5" ht="21.75" customHeight="1" spans="1:10">
       <c r="A5" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" s="10">
         <v>44704</v>
@@ -1468,7 +1471,7 @@
         <v>1</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F5" s="9"/>
       <c r="G5" s="10">
@@ -1478,13 +1481,13 @@
         <v>1</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="J5" s="23"/>
     </row>
     <row r="6" ht="22.5" customHeight="1" spans="1:10">
       <c r="A6" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B6" s="10">
         <v>44732</v>
@@ -1496,7 +1499,7 @@
         <v>0.9</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F6" s="9"/>
       <c r="G6" s="10">
@@ -1506,13 +1509,13 @@
         <v>0.9</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="J6" s="23"/>
     </row>
     <row r="7" ht="24.75" customHeight="1" spans="1:10">
       <c r="A7" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B7" s="10">
         <v>44737</v>
@@ -1524,7 +1527,7 @@
         <v>0.8</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F7" s="9"/>
       <c r="G7" s="10">
@@ -1534,13 +1537,13 @@
         <v>0.8</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="J7" s="23"/>
     </row>
     <row r="8" ht="22.5" customHeight="1" spans="1:10">
       <c r="A8" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B8" s="10">
         <v>44905</v>
@@ -1552,7 +1555,7 @@
         <v>1</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F8" s="9"/>
       <c r="G8" s="10">
@@ -1562,13 +1565,13 @@
         <v>1</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J8" s="23"/>
     </row>
     <row r="9" ht="25.5" customHeight="1" spans="1:10">
       <c r="A9" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
@@ -1582,7 +1585,7 @@
     </row>
     <row r="10" ht="24" customHeight="1" spans="1:10">
       <c r="A10" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
@@ -1596,7 +1599,7 @@
     </row>
     <row r="11" ht="24" customHeight="1" spans="1:10">
       <c r="A11" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
@@ -1610,7 +1613,7 @@
     </row>
     <row r="12" ht="21" customHeight="1" spans="1:10">
       <c r="A12" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
@@ -1624,7 +1627,7 @@
     </row>
     <row r="13" ht="19" customHeight="1" spans="1:10">
       <c r="A13" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B13" s="15"/>
       <c r="C13" s="15"/>

</xml_diff>

<commit_message>
fix and upload course
</commit_message>
<xml_diff>
--- a/DivisionOfWorl_BC35E_BTcapstone_Hau&Lanh.xlsx
+++ b/DivisionOfWorl_BC35E_BTcapstone_Hau&Lanh.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="34">
   <si>
     <t>Tasks Name</t>
   </si>
@@ -91,7 +91,10 @@
     <t>course</t>
   </si>
   <si>
-    <t>Dev A</t>
+    <t>24/8/2022</t>
+  </si>
+  <si>
+    <t>25/8/2022</t>
   </si>
   <si>
     <t>Nhật Trường</t>
@@ -126,10 +129,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="178" formatCode="[$-409]d\-mmm;@"/>
   </numFmts>
   <fonts count="28">
@@ -195,6 +198,20 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -211,56 +228,26 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -280,16 +267,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -303,37 +290,53 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -384,19 +387,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -408,7 +549,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -420,145 +561,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -721,26 +724,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -771,6 +754,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -794,18 +786,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -815,130 +818,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="25" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="13" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1341,7 +1344,7 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1533,17 +1536,17 @@
       <c r="A7" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="10">
-        <v>44737</v>
-      </c>
-      <c r="C7" s="10">
-        <v>44743</v>
+      <c r="B7" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>24</v>
       </c>
       <c r="D7" s="13">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="F7" s="9"/>
       <c r="G7" s="10">
@@ -1553,13 +1556,13 @@
         <v>0.8</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J7" s="24"/>
     </row>
     <row r="8" ht="22.5" customHeight="1" spans="1:10">
       <c r="A8" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B8" s="10">
         <v>44905</v>
@@ -1571,7 +1574,7 @@
         <v>1</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F8" s="9"/>
       <c r="G8" s="10">
@@ -1581,13 +1584,13 @@
         <v>1</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J8" s="24"/>
     </row>
     <row r="9" ht="25.5" customHeight="1" spans="1:10">
       <c r="A9" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
@@ -1601,7 +1604,7 @@
     </row>
     <row r="10" ht="24" customHeight="1" spans="1:10">
       <c r="A10" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
@@ -1615,7 +1618,7 @@
     </row>
     <row r="11" ht="24" customHeight="1" spans="1:10">
       <c r="A11" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
@@ -1629,7 +1632,7 @@
     </row>
     <row r="12" ht="21" customHeight="1" spans="1:10">
       <c r="A12" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
@@ -1643,7 +1646,7 @@
     </row>
     <row r="13" ht="19" customHeight="1" spans="1:10">
       <c r="A13" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B13" s="16"/>
       <c r="C13" s="16"/>

</xml_diff>